<commit_message>
Update zu einigen Dateien
</commit_message>
<xml_diff>
--- a/images/hallenbelegung.xlsx
+++ b/images/hallenbelegung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Klara\Desktop\Turnverein Weitersburg\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4EF21C-3753-4504-9714-C3CE93F9496C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045F9824-CA4E-493E-97B6-C93839180669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="85">
   <si>
     <t>Vereinseigene Halle</t>
   </si>
@@ -177,6 +177,9 @@
     <t>Kung Fu</t>
   </si>
   <si>
+    <t>Samstag</t>
+  </si>
+  <si>
     <t>Aquafitness</t>
   </si>
   <si>
@@ -216,12 +219,6 @@
     <t>Bodyfit</t>
   </si>
   <si>
-    <t>Zoll ab 9.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zoll </t>
-  </si>
-  <si>
     <t>8.00 - 9.00</t>
   </si>
   <si>
@@ -237,7 +234,7 @@
     <t>Christa-Herzog-Schule, CJD Engers</t>
   </si>
   <si>
-    <t>Polizei</t>
+    <t>Kung fu</t>
   </si>
   <si>
     <t>Rollsport</t>
@@ -258,29 +255,35 @@
     <t>Bodyworkout (Winter)</t>
   </si>
   <si>
-    <t>Hoop Fit</t>
-  </si>
-  <si>
     <t>Frauen Ika</t>
   </si>
   <si>
     <t>KiGaKids</t>
   </si>
   <si>
-    <t>Tanzen</t>
-  </si>
-  <si>
-    <t>Stand: Frühjahr 2022</t>
-  </si>
-  <si>
-    <t>Samstag</t>
+    <t>Fördergruppe Mädchen</t>
+  </si>
+  <si>
+    <t>Fördergruppe Jungen</t>
+  </si>
+  <si>
+    <t>Stand: Frühjahr 2023</t>
+  </si>
+  <si>
+    <t>Streetdance Erwachsene</t>
+  </si>
+  <si>
+    <t>Dance Kids</t>
+  </si>
+  <si>
+    <t>Dance Kids Minis (ab 14 Uhr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -315,9 +318,21 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
       <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -330,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -369,6 +384,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="double">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color indexed="8"/>
       </left>
@@ -471,6 +501,21 @@
       <left style="thin">
         <color indexed="8"/>
       </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="double">
+        <color indexed="8"/>
+      </top>
+      <bottom style="double">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
       <right/>
       <top style="double">
         <color indexed="8"/>
@@ -495,6 +540,34 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -506,6 +579,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -517,6 +599,30 @@
         <color indexed="8"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -531,6 +637,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="double">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color indexed="64"/>
       </left>
@@ -561,6 +682,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color indexed="64"/>
       </left>
@@ -587,6 +723,64 @@
       </top>
       <bottom style="double">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="double">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="double">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -626,6 +820,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="double">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -649,6 +856,17 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -709,41 +927,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -765,115 +948,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="double">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -882,10 +956,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -895,221 +968,189 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1453,446 +1494,439 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.54296875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" customWidth="1"/>
+    <col min="6" max="6" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="75" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
+      <c r="A2" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
     </row>
     <row r="4" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="78"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="62" t="s">
+      <c r="F5" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="77" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" s="2"/>
+      <c r="G5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="B6" s="42"/>
+      <c r="C6" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+        <v>54</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
+      <c r="B9" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+        <v>55</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+        <v>56</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="18"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="18"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="26"/>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="18"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="26"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="16" t="s">
+      <c r="B15" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="18"/>
+      <c r="D15" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="26"/>
       <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="53"/>
-      <c r="F16" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="18"/>
+      <c r="D16" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="26"/>
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="54"/>
-      <c r="F17" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="21"/>
+      <c r="D17" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="73"/>
+      <c r="F17" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="26"/>
       <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" s="21"/>
+      <c r="D18" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="26"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="20" t="s">
+      <c r="C19" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="21"/>
+      <c r="F19" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="26"/>
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="17" t="s">
+      <c r="C20" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="21"/>
+      <c r="F20" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="26"/>
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="17" t="s">
+      <c r="C21" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" s="18"/>
+      <c r="F21" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="26"/>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>63</v>
+      <c r="C22" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="18"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="26"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="22" t="s">
         <v>43</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="29"/>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="22" t="s">
         <v>43</v>
       </c>
       <c r="C24" s="22"/>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="18"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="30"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="22" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="22"/>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="18"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="30"/>
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23" t="s">
+      <c r="C26" s="31"/>
+      <c r="D26" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="79"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1902,391 +1936,336 @@
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="58" t="s">
+      <c r="A28" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="44"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:8" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="31"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="51"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="52" t="s">
+      <c r="E29" s="46"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="42" t="s">
+      <c r="B30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="38"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="57"/>
+    </row>
+    <row r="31" spans="1:8" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="47"/>
-      <c r="D31" s="42" t="s">
+      <c r="B31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="38"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="57"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="52" t="s">
+    <row r="32" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="42" t="s">
+      <c r="B32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="39"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="57"/>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="39"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="56"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="57"/>
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="E34" s="38"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="38"/>
+      <c r="D34" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="56"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="57"/>
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" s="66" t="s">
+      <c r="D35" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="39"/>
+      <c r="G35" s="57"/>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="53" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="38" t="s">
+      <c r="D36" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="57"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="43" t="s">
+      <c r="F37" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="39"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="43" t="s">
+      <c r="G37" s="57"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="38" t="s">
+      <c r="E38" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="43" t="s">
+      <c r="F38" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="38"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="38"/>
+      <c r="G38" s="57"/>
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="53" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="66" t="s">
         <v>46</v>
       </c>
       <c r="E39" s="8"/>
-      <c r="F39" s="43" t="s">
+      <c r="F39" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="38"/>
+      <c r="G39" s="57"/>
       <c r="H39" s="6"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="53" t="s">
         <v>35</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="37" t="s">
+      <c r="D40" s="66" t="s">
         <v>46</v>
       </c>
       <c r="E40" s="8"/>
-      <c r="F40" s="43" t="s">
+      <c r="F40" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="G40" s="38"/>
+      <c r="G40" s="57"/>
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="53" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="37" t="s">
+      <c r="D41" s="66" t="s">
         <v>46</v>
       </c>
       <c r="E41" s="8"/>
-      <c r="F41" s="43" t="s">
+      <c r="F41" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="G41" s="38"/>
+      <c r="G41" s="57"/>
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41" t="s">
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="41"/>
-      <c r="F42" s="67" t="s">
+      <c r="E42" s="61"/>
+      <c r="F42" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="G42" s="27"/>
+      <c r="G42" s="63"/>
     </row>
     <row r="43" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="71"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="73"/>
+      <c r="A43" s="70"/>
+      <c r="B43" s="71"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="61"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
+      <c r="A44" s="45"/>
     </row>
     <row r="45" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="59" t="s">
+      <c r="A45" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="44"/>
     </row>
     <row r="46" spans="1:8" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15" t="s">
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="80"/>
-    </row>
-    <row r="47" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-    </row>
+      <c r="E46" s="13"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:8" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="44"/>
+      <c r="A48" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="49" spans="1:7" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
+    </row>
+    <row r="50" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="38"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="40"/>
+    </row>
+    <row r="51" spans="1:7" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="27"/>
-    </row>
-    <row r="51" spans="1:7" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-    </row>
-    <row r="52" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" s="44"/>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-    </row>
-    <row r="53" spans="1:7" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="50" t="s">
+      <c r="B53" s="13"/>
+      <c r="C53" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="14"/>
+    </row>
+    <row r="54" spans="1:7" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="51"/>
-      <c r="C53" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="51"/>
-    </row>
-    <row r="54" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="69"/>
-      <c r="G54" s="27"/>
-    </row>
-    <row r="55" spans="1:7" ht="13" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
+      <c r="C54" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A43:G43"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -2303,9 +2282,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="11" style="1"/>
-  </cols>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.49236111111111114" footer="0.49236111111111114"/>
@@ -2321,9 +2297,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="11" style="1"/>
-  </cols>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.49236111111111114" footer="0.49236111111111114"/>

</xml_diff>